<commit_message>
Fix timeout issue in container
</commit_message>
<xml_diff>
--- a/data/gold_standard.xlsx
+++ b/data/gold_standard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MastersThesis\UseCase\ma-use-case\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78388316-8B84-4E27-A62E-51BCB3471D2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7349EC-E2F8-41F7-B360-CACB7F581407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="300" windowWidth="38730" windowHeight="21330" xr2:uid="{3A0255F1-C9CF-4400-BB4D-4447490A81F1}"/>
+    <workbookView xWindow="25490" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{3A0255F1-C9CF-4400-BB4D-4447490A81F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -105,9 +105,6 @@
     <t>I do not understand Governatories formalism here. It seems to me like the generated output is bettr?</t>
   </si>
   <si>
-    <t>Chatper 8.2.1 (a) (ii) of Autralian Telecommunications Consumer Protections Code (Aided by the formalism in https://github.com/DasElias/LLM-DDL-NLP/blob/main/Experiment_2_3/evaluation_output_deepseek-r1.xml)</t>
-  </si>
-  <si>
     <t>:- dynamic complaint_in_person/1.
 :- dynamic complaint_by_telephone/1.
 :- dynamic complaint_by_email/1.
@@ -478,6 +475,9 @@
   </si>
   <si>
     <t>AVG</t>
+  </si>
+  <si>
+    <t>Chatper 8.2.1 (a) (ii) of Australian Telecommunications Consumer Protections Code (Aided by the formalism in https://github.com/DasElias/LLM-DDL-NLP/blob/main/Experiment_2_3/evaluation_output_deepseek-r1.xml)</t>
   </si>
 </sst>
 </file>
@@ -968,8 +968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7942F073-5A1B-4C73-B1E9-BA20EE3B78CE}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,21 +999,21 @@
         <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="390" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -1025,114 +1025,114 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="270" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>99</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="330" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>23</v>
-      </c>
       <c r="G6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1161,24 +1161,24 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>48</v>
-      </c>
-      <c r="E1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1192,7 +1192,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1206,7 +1206,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1218,12 +1218,12 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1237,7 +1237,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1251,7 +1251,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1263,12 +1263,12 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1320,21 +1320,21 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>47</v>
-      </c>
-      <c r="D1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1348,7 +1348,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1362,7 +1362,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1376,7 +1376,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1390,7 +1390,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1404,7 +1404,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1418,7 +1418,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1432,7 +1432,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1444,12 +1444,12 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1461,12 +1461,12 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1478,12 +1478,12 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1497,7 +1497,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1509,7 +1509,7 @@
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1553,21 +1553,21 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>47</v>
-      </c>
-      <c r="D1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1581,7 +1581,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1595,7 +1595,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1607,12 +1607,12 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1626,7 +1626,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1640,7 +1640,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1683,21 +1683,21 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>47</v>
-      </c>
-      <c r="D1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1711,7 +1711,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1725,7 +1725,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1739,7 +1739,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1753,7 +1753,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1767,7 +1767,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1781,7 +1781,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1795,7 +1795,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H9" t="s">
         <v>10</v>
@@ -1819,7 +1819,7 @@
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1842,21 +1842,21 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>47</v>
-      </c>
-      <c r="D1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1868,12 +1868,12 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1885,12 +1885,12 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1902,12 +1902,12 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1919,12 +1919,12 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1938,7 +1938,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1950,12 +1950,12 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1969,7 +1969,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1981,18 +1981,18 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H11" t="s">
+        <v>90</v>
+      </c>
+      <c r="I11" t="s">
         <v>91</v>
-      </c>
-      <c r="I11" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2022,7 +2022,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2048,22 +2048,22 @@
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" t="s">
         <v>94</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>95</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>96</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>97</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>98</v>
-      </c>
-      <c r="I1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>